<commit_message>
commit chapter 5 to key notes
</commit_message>
<xml_diff>
--- a/PMP/PMP_Keynotes.xlsx
+++ b/PMP/PMP_Keynotes.xlsx
@@ -5,14 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hdeng\Documents\GitHub\documents\PMP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HDENG\Documents\github\documents\PMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4090"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="4095" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ProcessDef" sheetId="1" r:id="rId1"/>
+    <sheet name="input" sheetId="2" r:id="rId2"/>
+    <sheet name="tech" sheetId="4" r:id="rId3"/>
+    <sheet name="output" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="159">
   <si>
     <t>制定项目章程</t>
   </si>
@@ -306,18 +309,446 @@
   </si>
   <si>
     <t>规划人力资源管理</t>
+  </si>
+  <si>
+    <t>项目工作说明书</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4.1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>制定项目章程</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>商业论证</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>协议（合同）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>事业环境因素</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>组织工程资产</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>项目章程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>项目管理子计划</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4.2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>制定项目管理计划</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>项目管理计划</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>批准的变更请求</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4.3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>指导与管理项目工作</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>进度预测</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>成本预测</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>确认的变更</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工作绩效信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>组织过程资产</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.4 监控项目工作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4.5 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>实施整体变更控制</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工作绩效报告</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>变更请求</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>变更请求</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4.6 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>结束项目或阶段</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>验收的可交付成果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>验收的可交付成果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>专家判断</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>引导技术</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>项目管理信息系统</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>会议</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分析技术</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>变更控制工具</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>项目章程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可交付成果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工作绩效数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工作绩效数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>项目管理计划更新</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>项目管理计划更新</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>项目文件更新</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>项目文件更新</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工作绩效报告</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>批准的变更请求</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>变更日志</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最终产品、服务或成果移交</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>组织过程资产更新</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">5.1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>规划范围管理</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>范围管理计划</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>需求管理计划</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>干系人管理计划</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>干系人登记册</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">5.2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>收集需求</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">5.3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>定义范围</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>需求文件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">5.4 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>创建</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WBS</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>项目范围说明书</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>需求跟踪矩阵</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>核实的可交付成果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">5.5 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>确认范围</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">5.6 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>控制范围</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>范围基准</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>访谈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>焦点小组</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>引导式研讨会</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>群体创新技术</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>群体决策技术</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>问卷调查</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -356,7 +787,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -365,6 +796,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,22 +1113,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="20.81640625" customWidth="1"/>
-    <col min="2" max="2" width="97.54296875" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="20.875" customWidth="1"/>
+    <col min="2" max="2" width="97.5" customWidth="1"/>
+    <col min="3" max="3" width="8.75" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -704,7 +1136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -712,7 +1144,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -720,7 +1152,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -728,7 +1160,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="28.5">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -736,7 +1168,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -744,11 +1176,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -756,7 +1188,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -764,7 +1196,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -772,7 +1204,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -780,7 +1212,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -788,7 +1220,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
@@ -796,11 +1228,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -808,7 +1240,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
@@ -816,7 +1248,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
         <v>29</v>
       </c>
@@ -824,7 +1256,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
         <v>31</v>
       </c>
@@ -832,7 +1264,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
         <v>85</v>
       </c>
@@ -840,7 +1272,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
         <v>33</v>
       </c>
@@ -848,7 +1280,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
         <v>36</v>
       </c>
@@ -856,11 +1288,11 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
         <v>38</v>
       </c>
@@ -868,7 +1300,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
         <v>40</v>
       </c>
@@ -876,7 +1308,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
         <v>42</v>
       </c>
@@ -884,7 +1316,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
         <v>44</v>
       </c>
@@ -892,11 +1324,11 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
         <v>46</v>
       </c>
@@ -904,7 +1336,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
         <v>48</v>
       </c>
@@ -912,7 +1344,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
         <v>50</v>
       </c>
@@ -920,11 +1352,11 @@
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
         <v>93</v>
       </c>
@@ -932,7 +1364,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
         <v>92</v>
       </c>
@@ -940,7 +1372,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
         <v>91</v>
       </c>
@@ -948,7 +1380,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
         <v>90</v>
       </c>
@@ -956,11 +1388,11 @@
         <v>89</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
         <v>82</v>
       </c>
@@ -968,7 +1400,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
         <v>83</v>
       </c>
@@ -976,7 +1408,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
         <v>84</v>
       </c>
@@ -984,11 +1416,11 @@
         <v>81</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
         <v>77</v>
       </c>
@@ -996,7 +1428,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
         <v>76</v>
       </c>
@@ -1004,7 +1436,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
         <v>73</v>
       </c>
@@ -1012,7 +1444,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
         <v>72</v>
       </c>
@@ -1020,7 +1452,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
         <v>70</v>
       </c>
@@ -1028,7 +1460,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
         <v>68</v>
       </c>
@@ -1036,11 +1468,11 @@
         <v>67</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
         <v>66</v>
       </c>
@@ -1048,7 +1480,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
         <v>63</v>
       </c>
@@ -1056,7 +1488,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
         <v>62</v>
       </c>
@@ -1064,7 +1496,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
         <v>59</v>
       </c>
@@ -1072,11 +1504,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
     </row>
-    <row r="54" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" ht="28.5">
       <c r="A54" s="2" t="s">
         <v>52</v>
       </c>
@@ -1084,7 +1516,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" ht="28.5">
       <c r="A55" s="2" t="s">
         <v>53</v>
       </c>
@@ -1092,7 +1524,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" ht="28.5">
       <c r="A56" s="2" t="s">
         <v>58</v>
       </c>
@@ -1100,7 +1532,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2">
       <c r="A57" s="1" t="s">
         <v>57</v>
       </c>
@@ -1109,7 +1541,805 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:B68"/>
+  <sheetViews>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="16.625" customWidth="1"/>
+    <col min="2" max="2" width="23.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2">
+      <c r="A2" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="4"/>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="4"/>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="4"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="4"/>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="4"/>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B32" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B36" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B41" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B47" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B52" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B58" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B64" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:B46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="17.125" customWidth="1"/>
+    <col min="2" max="2" width="21.75" customWidth="1"/>
+    <col min="3" max="3" width="26.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2">
+      <c r="A2" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="4"/>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="4"/>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="4"/>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="4"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="4"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B25" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B28" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="B35" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="B38" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="B41" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="B46" t="s">
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:B47"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25:B43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="25.375" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2">
+      <c r="A2" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="4"/>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="4"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B17" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="4"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B25" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B28" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B31" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B34" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B37" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="4"/>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B42" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="4"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>